<commit_message>
improved UI and design in stats, filters and added some stuff to scrum report
</commit_message>
<xml_diff>
--- a/src/main/resources/iteration2_scrumReport_wolf.xlsx
+++ b/src/main/resources/iteration2_scrumReport_wolf.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9A8C0549-3CC1-4F9E-9FD1-F006BE0E8A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6F35A833-5842-4EA0-B2FA-B9C0CF7BB4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="100">
   <si>
     <t>Iteration</t>
   </si>
@@ -307,6 +307,15 @@
   </si>
   <si>
     <t>Centralized global UI theme (colors, fonts, components) using shared CSS across all views.</t>
+  </si>
+  <si>
+    <t>Enhanced History filtering with smart free-text inference and separated filtering logic from the UI controller.</t>
+  </si>
+  <si>
+    <t>The History screen now infers filter intent (Result, Difficulty, or Player Name) when the filter type remains “All”, applies strict validation for result keywords, and keeps date filtering explicit. Filtering and validation logic were moved to a dedicated service to improve code clarity, testability, and maintainability.</t>
+  </si>
+  <si>
+    <t>Improved settings toggles by replacing ToggleButtons with image-based switches for clearer visual feedback.</t>
   </si>
 </sst>
 </file>
@@ -874,8 +883,8 @@
   <dimension ref="A1:I1016"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G52" sqref="G52"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F52" sqref="F52:G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1910,20 +1919,42 @@
     </row>
     <row r="51" spans="1:9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="7"/>
+      <c r="B51" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="52" spans="1:9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
+      <c r="B52" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="G52" s="7"/>
     </row>
     <row r="53" spans="1:9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>